<commit_message>
Report format changes on BA rpt and Loan rpt.
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/BAReport/BAReport.xlsx
+++ b/Src/SummitReports.Objects/Reports/BAReport/BAReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajoyce\Documents\GitHub\SummitReports\Src\SummitReports.Objects\Reports\BAReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2FAF93-7949-4E70-9108-78B1933ACAB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7420CAC3-D052-4F5B-911E-ABAC83AF5F53}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21585" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="17280" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -554,8 +554,8 @@
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>

</xml_diff>